<commit_message>
Worked on Excel Data Analysis chapter 3-5
</commit_message>
<xml_diff>
--- a/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter04/Binomial.xlsx
+++ b/LinkedIn/Excel_Data_Analysis/Exercise Files/Chapter04/Binomial.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Desktop\Exercise Files\Chapter04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtalebiz\Desktop\Jupyter\Examples\LinkedIn\Excel_Data_Analysis\Exercise Files\Chapter04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4106F08-BCB6-431A-9201-12C811724CF5}" xr6:coauthVersionLast="39" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B3C29A-1187-4836-BDCA-8674DC50BC0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10965" yWindow="3210" windowWidth="19560" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binomial" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -345,67 +351,67 @@
                 <c:formatCode>0.0000000000%</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.9485158708621573E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.6145272065469201E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.15117247776640336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.32891082587567666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.54196897392974175</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.73426761012212838</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.86986280230906765</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.9463523979017</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.98141012921498982</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.99459423329862018</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.99868468610405414</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.99973352015672967</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.99995538889864166</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.99999389866055144</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.99999932952441051</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.99999994223725619</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>0.99999999624239488</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>0.99999999982644627</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>0.99999999999492739</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>0.99999999999992939</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1200,7 +1206,9 @@
   <autoFilter ref="A4:B25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Successes"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percentage of Outcomes" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Percentage of Outcomes" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>_xlfn.BINOM.DIST(A5, $B$2, $B$1,TRUE)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1531,7 +1539,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1581,8 @@
         <v>0</v>
       </c>
       <c r="B5" s="4">
-        <v>0</v>
+        <f t="shared" ref="B5:B25" si="0">_xlfn.BINOM.DIST(A5, $B$2, $B$1,TRUE)</f>
+        <v>6.9485158708621573E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1581,7 +1590,8 @@
         <v>1</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4.6145272065469201E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1589,7 +1599,8 @@
         <v>2</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.15117247776640336</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1597,7 +1608,8 @@
         <v>3</v>
       </c>
       <c r="B8" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.32891082587567666</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,7 +1617,8 @@
         <v>4</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.54196897392974175</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1626,8 @@
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.73426761012212838</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1621,7 +1635,8 @@
         <v>6</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.86986280230906765</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,7 +1644,8 @@
         <v>7</v>
       </c>
       <c r="B12" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.9463523979017</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1637,7 +1653,8 @@
         <v>8</v>
       </c>
       <c r="B13" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.98141012921498982</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1645,7 +1662,8 @@
         <v>9</v>
       </c>
       <c r="B14" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99459423329862018</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1653,7 +1671,8 @@
         <v>10</v>
       </c>
       <c r="B15" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99868468610405414</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1661,7 +1680,8 @@
         <v>11</v>
       </c>
       <c r="B16" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99973352015672967</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +1689,8 @@
         <v>12</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99995538889864166</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,7 +1698,8 @@
         <v>13</v>
       </c>
       <c r="B18" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999389866055144</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +1707,8 @@
         <v>14</v>
       </c>
       <c r="B19" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999932952441051</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,7 +1716,8 @@
         <v>15</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999994223725619</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +1725,8 @@
         <v>16</v>
       </c>
       <c r="B21" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999624239488</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +1734,8 @@
         <v>17</v>
       </c>
       <c r="B22" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999982644627</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,7 +1743,8 @@
         <v>18</v>
       </c>
       <c r="B23" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999492739</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1752,8 @@
         <v>19</v>
       </c>
       <c r="B24" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999992939</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +1761,8 @@
         <v>20</v>
       </c>
       <c r="B25" s="4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>